<commit_message>
Updated forecast file formatting
</commit_message>
<xml_diff>
--- a/2018SuperRugby/Weekly Forecasts/Round_SF.xlsx
+++ b/2018SuperRugby/Weekly Forecasts/Round_SF.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RugbyPredictifier\2018SuperRugby\Weekly Forecasts\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Saturday" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>City</t>
   </si>
@@ -121,14 +127,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#0.00"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="#0%"/>
     <numFmt numFmtId="167" formatCode="#0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,17 +251,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -263,6 +269,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -309,7 +323,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -341,9 +355,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -375,6 +407,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -550,7 +600,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
@@ -558,9 +608,16 @@
       <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="1.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:61">
+    <row r="1" spans="1:61" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
@@ -583,523 +640,451 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:61">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="6"/>
-      <c r="E2" s="6" t="s">
+      <c r="C2" s="8"/>
+      <c r="E2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="6"/>
-    </row>
-    <row r="3" spans="1:61">
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="7">
-        <v>0.9236663418771702</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="E3" s="7">
+      <c r="B3" s="9">
+        <v>0.92366634187717023</v>
+      </c>
+      <c r="C3" s="9"/>
+      <c r="E3" s="9">
         <v>0.7399221465969158</v>
       </c>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:61">
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="7">
-        <v>0.9128704364219197</v>
-      </c>
-      <c r="C4" s="7"/>
-      <c r="E4" s="7">
-        <v>0.9946385979525496</v>
-      </c>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:61">
+      <c r="B4" s="9">
+        <v>0.91287043642191967</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="E4" s="9">
+        <v>0.99463859795254961</v>
+      </c>
+      <c r="F4" s="9"/>
+    </row>
+    <row r="5" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6">
-        <v>84.31876966176505</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="E5" s="6">
+      <c r="B5" s="8">
+        <v>84.318769661765046</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="E5" s="8">
         <v>73.59551264851973</v>
       </c>
-      <c r="F5" s="6"/>
-    </row>
-    <row r="6" spans="1:61">
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="8">
-        <v>0.6719995</v>
-      </c>
-      <c r="C6" s="8">
-        <v>0.3280005</v>
-      </c>
-      <c r="E6" s="8">
-        <v>0.5430792</v>
-      </c>
-      <c r="F6" s="8">
-        <v>0.4569208</v>
-      </c>
-    </row>
-    <row r="7" spans="1:61">
+      <c r="B6" s="6">
+        <v>0.67199949999999997</v>
+      </c>
+      <c r="C6" s="6">
+        <v>0.32800049999999997</v>
+      </c>
+      <c r="E6" s="6">
+        <v>0.54307919999999998</v>
+      </c>
+      <c r="F6" s="6">
+        <v>0.45692080000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="9">
-        <v>32.9864874</v>
-      </c>
-      <c r="C7" s="9">
-        <v>23.8915832</v>
-      </c>
-      <c r="E7" s="9">
-        <v>39.8903092</v>
-      </c>
-      <c r="F7" s="9">
-        <v>37.3147208</v>
-      </c>
-    </row>
-    <row r="8" spans="1:61">
+      <c r="B7" s="7">
+        <v>32.986487400000001</v>
+      </c>
+      <c r="C7" s="7">
+        <v>23.891583199999999</v>
+      </c>
+      <c r="E7" s="7">
+        <v>39.890309199999997</v>
+      </c>
+      <c r="F7" s="7">
+        <v>37.314720800000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="9">
+      <c r="B8" s="7">
         <v>9</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>6</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="7">
         <v>14</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="7">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:61">
+    <row r="9" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>14</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>8</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="7">
         <v>19</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="7">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:61">
+    <row r="10" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="9">
+      <c r="B10" s="7">
         <v>16</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>11</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="7">
         <v>22</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="7">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:61">
+    <row r="11" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="9">
+      <c r="B11" s="7">
         <v>19</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>14</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="7">
         <v>24</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="7">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:61">
+    <row r="12" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B12" s="7">
         <v>22</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>14</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="7">
         <v>28</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="7">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:61">
+    <row r="13" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="9">
+      <c r="B13" s="7">
         <v>24</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="7">
         <v>16</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="7">
         <v>30</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="7">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:61">
+    <row r="14" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9">
+      <c r="B14" s="7">
         <v>25</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="7">
         <v>17</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="7">
         <v>32</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="7">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:61">
+    <row r="15" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="7">
         <v>28</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="7">
         <v>19</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="7">
         <v>34</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="7">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="1:61">
+    <row r="16" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="9">
+      <c r="B16" s="7">
         <v>30</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="7">
         <v>22</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="7">
         <v>36</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="9">
+      <c r="B17" s="7">
         <v>32</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="7">
         <v>22</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="7">
         <v>38</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="7">
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="7">
         <v>33</v>
       </c>
-      <c r="C18" s="9">
+      <c r="C18" s="7">
         <v>24</v>
       </c>
-      <c r="E18" s="9">
+      <c r="E18" s="7">
         <v>41</v>
       </c>
-      <c r="F18" s="9">
+      <c r="F18" s="7">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="9">
+      <c r="B19" s="7">
         <v>36</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <v>26</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="7">
         <v>43</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="7">
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="9">
+      <c r="B20" s="7">
         <v>38</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <v>28</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="7">
         <v>46</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="7">
         <v>43</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="9">
+      <c r="B21" s="7">
         <v>40</v>
       </c>
-      <c r="C21" s="9">
+      <c r="C21" s="7">
         <v>30</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="7">
         <v>48</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21" s="7">
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="9">
+      <c r="B22" s="7">
         <v>43</v>
       </c>
-      <c r="C22" s="9">
+      <c r="C22" s="7">
         <v>32</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="7">
         <v>51</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F22" s="7">
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="9">
+      <c r="B23" s="7">
         <v>46</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="7">
         <v>34</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="7">
         <v>54</v>
       </c>
-      <c r="F23" s="9">
+      <c r="F23" s="7">
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="9">
+      <c r="B24" s="7">
         <v>49</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="7">
         <v>38</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="7">
         <v>58</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="7">
         <v>54</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="9">
+      <c r="B25" s="7">
         <v>54</v>
       </c>
-      <c r="C25" s="9">
+      <c r="C25" s="7">
         <v>41</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="7">
         <v>62</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="7">
         <v>59</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="9">
+      <c r="B26" s="7">
         <v>60</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="7">
         <v>47</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="7">
         <v>70</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="7">
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="8">
+      <c r="B27" s="6">
         <v>0.2897248</v>
       </c>
-      <c r="C27" s="8">
-        <v>0.083022</v>
-      </c>
-      <c r="E27" s="8">
-        <v>0.3033852</v>
-      </c>
-      <c r="F27" s="8">
+      <c r="C27" s="6">
+        <v>8.3021999999999999E-2</v>
+      </c>
+      <c r="E27" s="6">
+        <v>0.30338520000000002</v>
+      </c>
+      <c r="F27" s="6">
         <v>0.1235772</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="8">
+      <c r="B28" s="6">
         <v>0.1093172</v>
       </c>
-      <c r="C28" s="8">
-        <v>0.129006</v>
-      </c>
-      <c r="E28" s="8">
+      <c r="C28" s="6">
+        <v>0.12900600000000001</v>
+      </c>
+      <c r="E28" s="6">
         <v>0.108351</v>
       </c>
-      <c r="F28" s="8">
+      <c r="F28" s="6">
         <v>0.1132358</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="152">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:C5"/>
+  <mergeCells count="8">
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:C4"/>
@@ -1108,78 +1093,6 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E5:F5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>